<commit_message>
Regression Update 10-04-19 with test output
</commit_message>
<xml_diff>
--- a/src/test/resources/docs/BankFileTest.xlsx
+++ b/src/test/resources/docs/BankFileTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DRC Merge Regreation\DRC-Automation\src\test\resources\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1253938-DEA1-4264-A7D1-6C7C4151A8C7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C1F518-D3B5-4A27-825E-821F4361B304}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CF704FE-2400-465E-B060-6F37E9B3C5EC}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Bank Name:</t>
   </si>
@@ -138,57 +138,44 @@
     <t>Advans Bank</t>
   </si>
   <si>
-    <t>00112233440037</t>
-  </si>
-  <si>
     <t>1600.00</t>
   </si>
   <si>
-    <t>FT19031400020</t>
-  </si>
-  <si>
-    <t>20190311070746381</t>
-  </si>
-  <si>
-    <t>smokeatuser61</t>
-  </si>
-  <si>
-    <t>FT1903140002A</t>
-  </si>
-  <si>
-    <t>20190311070746381A</t>
-  </si>
-  <si>
-    <t>15-03-2019 11:18:40</t>
-  </si>
-  <si>
-    <t>502916.70</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>16-03-2019 16:25:27</t>
-  </si>
-  <si>
-    <t>FT19031600001</t>
-  </si>
-  <si>
-    <t>FT1903160000A</t>
-  </si>
-  <si>
-    <t>2019031107074638A</t>
-  </si>
-  <si>
-    <t>FT1903160000B</t>
+    <t>09-04-2019 12:18:09</t>
+  </si>
+  <si>
+    <t>FT19040900002</t>
+  </si>
+  <si>
+    <t>20190408110339126</t>
+  </si>
+  <si>
+    <t>00112233440042</t>
+  </si>
+  <si>
+    <t>Regression AprilOne</t>
+  </si>
+  <si>
+    <t>FT1904090000X</t>
+  </si>
+  <si>
+    <t>2019040811033912X</t>
+  </si>
+  <si>
+    <t>FT1904090000Y</t>
+  </si>
+  <si>
+    <t>FT1904090000Z</t>
+  </si>
+  <si>
+    <t>1610</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,22 +569,22 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +595,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -653,85 +640,107 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
       </c>
       <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
         <v>13</v>
       </c>
       <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
       </c>
       <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>